<commit_message>
EN COURS - task references #131: Mise à jour des requetes dans logindatase.cpp suite maj de la base http://gestion.xsilium.com/issues/131
</commit_message>
<xml_diff>
--- a/src/server/Shared/Databases/liste des requetes.xlsx
+++ b/src/server/Shared/Databases/liste des requetes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="57">
   <si>
     <t>Nom requete</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>LOGIN_SET_EXPIREDACCBANS</t>
+  </si>
+  <si>
+    <t>REALMS_INS_BANIP_BANAUTOIP</t>
+  </si>
+  <si>
+    <t>Ban auto de l'ip pour erreur authentification</t>
+  </si>
+  <si>
+    <t>INSERT INTO ip_banned VALUES ($1, now(), now() + INTERVAL  '20 minute', 'AutoBan pour erreur authentification ', $2, true)</t>
   </si>
 </sst>
 </file>
@@ -529,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,6 +789,23 @@
       </c>
       <c r="E14" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EN COURS - task references #133: Creation ip_temporaire http://gestion.xsilium.com/issues/133
</commit_message>
<xml_diff>
--- a/src/server/Shared/Databases/liste des requetes.xlsx
+++ b/src/server/Shared/Databases/liste des requetes.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
   <si>
     <t>Nom requete</t>
   </si>
@@ -271,6 +271,57 @@
   </si>
   <si>
     <t>REALMS_SEL_AVERTISSEMENTS_LISTEAVERTOS</t>
+  </si>
+  <si>
+    <t>REALMS_INS_IPTEMPORAIRE_STOCKAGEIPTEMPORAIRE</t>
+  </si>
+  <si>
+    <t>REALMS_UPD_IPTEMPORAIRE_MAJIPTEMPORAIRE</t>
+  </si>
+  <si>
+    <t>REALMS_SEL_IPTEMPORAIRE_LECTURENERREURS</t>
+  </si>
+  <si>
+    <t>REALMS_SEL_IPTEMPORAIRE_RECHERCHEIP</t>
+  </si>
+  <si>
+    <t>REALMS_DEL_IPTEMPORAIRE_SUPPRLIGNEIP</t>
+  </si>
+  <si>
+    <t>ip_temporaire</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>Création d'une erreur d'authentification sur une nouvelle ip</t>
+  </si>
+  <si>
+    <t>Création d'une erreur d'authentification sur une ip existante</t>
+  </si>
+  <si>
+    <t>Lecteure du nombre d'erreurs d'authentification sur une ip</t>
+  </si>
+  <si>
+    <t>Savoir si une ip a déjà eu une erreur d'authentification</t>
+  </si>
+  <si>
+    <t>Suppression des lignes sans erreurs d'authentification</t>
+  </si>
+  <si>
+    <t>INSERT INTO ip_temporaire VALUES ($1, '1')</t>
+  </si>
+  <si>
+    <t>UPDATE ip_temporaire SET ip_temp_nessais = $1 WHERE ip_temp_ip = $2"</t>
+  </si>
+  <si>
+    <t>SELECT ip_temp_nessais FROM ip_temporaire where ip_temp_ip = $1</t>
+  </si>
+  <si>
+    <t>SELECT ip_temp_ip FROM ip_temporaire where ip_temp_ip = $1</t>
+  </si>
+  <si>
+    <t>DELETE FROM ip_temporaire where ip_temp_nessais = '0'</t>
   </si>
 </sst>
 </file>
@@ -619,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,6 +1091,91 @@
       </c>
       <c r="E24" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>95</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incomplete - task references #131: Mise à jour des requetes dans logindatase.cpp suite maj de la base http://gestion.snowsuprem.eu/issues/show/131
</commit_message>
<xml_diff>
--- a/src/server/Shared/Databases/liste des requetes.xlsx
+++ b/src/server/Shared/Databases/liste des requetes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="80" windowWidth="20120" windowHeight="8000"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,19 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$E$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$E$29</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="101">
   <si>
     <t>Nom requete</t>
   </si>
@@ -282,9 +287,6 @@
     <t>REALMS_SEL_IPTEMPORAIRE_LECTURENERREURS</t>
   </si>
   <si>
-    <t>REALMS_SEL_IPTEMPORAIRE_RECHERCHEIP</t>
-  </si>
-  <si>
     <t>REALMS_DEL_IPTEMPORAIRE_SUPPRLIGNEIP</t>
   </si>
   <si>
@@ -303,9 +305,6 @@
     <t>Lecteure du nombre d'erreurs d'authentification sur une ip</t>
   </si>
   <si>
-    <t>Savoir si une ip a déjà eu une erreur d'authentification</t>
-  </si>
-  <si>
     <t>Suppression des lignes sans erreurs d'authentification</t>
   </si>
   <si>
@@ -316,9 +315,6 @@
   </si>
   <si>
     <t>SELECT ip_temp_nessais FROM ip_temporaire where ip_temp_ip = $1</t>
-  </si>
-  <si>
-    <t>SELECT ip_temp_ip FROM ip_temporaire where ip_temp_ip = $1</t>
   </si>
   <si>
     <t>DELETE FROM ip_temporaire where ip_temp_nessais = '0'</t>
@@ -337,7 +333,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,6 +344,22 @@
     <font>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -370,8 +382,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -379,7 +399,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -679,22 +707,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.5" customWidth="1"/>
     <col min="5" max="5" width="109" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -711,7 +740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -728,7 +757,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -745,7 +774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -762,7 +791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -779,7 +808,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -796,7 +825,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -813,7 +842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -830,7 +859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -847,7 +876,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -864,7 +893,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -881,7 +910,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -898,7 +927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -915,7 +944,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -932,7 +961,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -949,7 +978,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -966,7 +995,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -983,7 +1012,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1000,7 +1029,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1017,7 +1046,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1034,7 +1063,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1051,7 +1080,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1068,7 +1097,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1085,7 +1114,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1102,9 +1131,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" t="s">
         <v>12</v>
@@ -1113,15 +1142,15 @@
         <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -1130,15 +1159,15 @@
         <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
         <v>10</v>
@@ -1147,67 +1176,62 @@
         <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" t="s">
         <v>89</v>
-      </c>
-      <c r="B28" t="s">
-        <v>10</v>
       </c>
       <c r="C28" t="s">
         <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E28" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" hidden="1">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" t="s">
-        <v>90</v>
-      </c>
-      <c r="C29" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" t="s">
-        <v>95</v>
       </c>
       <c r="E29" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" t="s">
-        <v>102</v>
-      </c>
-      <c r="E30" t="s">
-        <v>103</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E24"/>
+  <autoFilter ref="A1:E29">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="ip_banned"/>
+        <filter val="ip_temporaire"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1217,9 +1241,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1229,8 +1258,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>